<commit_message>
Extended Unit Tests to support Indentity Inserts
</commit_message>
<xml_diff>
--- a/UT.Vend.BLL/HelperFiles/Project.xlsx
+++ b/UT.Vend.BLL/HelperFiles/Project.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>ProjectID</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>[Vend].[tblProject]</t>
   </si>
 </sst>
 </file>
@@ -530,264 +536,297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.125" customWidth="1"/>
-    <col min="3" max="3" width="23.375" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="23.375" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="str">
-        <f>"INSERT INTO [Vend].[tblProject] ([" &amp; A$1 &amp;"],["&amp;B$1&amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; A2 &amp; "','" &amp; B2 &amp; "','" &amp; C2 &amp; "' )"</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"INSERT INTO "&amp;A2&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "' )"</f>
         <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( 'f79359bb-2524-4cd5-b452-acaa8fd0d33b','Scorpion Cloudy','Lorem ipsum dolor sit amet, consectetur adipiscing elit.' )</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F11" si="0">"INSERT INTO [Vend].[tblProject] ([" &amp; A$1 &amp;"],["&amp;B$1&amp;"],["&amp;C$1&amp;"]) VALUES ( '" &amp; A3 &amp; "','" &amp; B3 &amp; "','" &amp; C3 &amp; "' )"</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G11" si="0">"INSERT INTO "&amp;A3&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "','" &amp; D3 &amp; "' )"</f>
         <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( '5cc9ad09-3002-40e8-8a30-96b656a9d805','Minimum Bulldozer','Praesent varius dolor quis sollicitudin ornare.' )</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="str">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( '54dbcf7a-0328-4a8d-9562-7d8c8b0c930b','Grotesque Viper','Duis a neque ac est fermentum rhoncus ac sed quam.' )</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="str">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( '364ac77c-d08e-4134-9849-fe731b00af2d','Wild Oyster','Sed ac quam vulputate, consectetur libero in, rutrum justo.' )</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="str">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( '25c7f719-8bde-447c-9b53-226c612de0bb','Third Temporary Hook','Nunc nec ipsum vitae ligula rutrum laoreet.' )</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="str">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( 'fb986b83-d3c1-4dc6-bb25-4ddc3423fd5e','Mysterious Fish','Nam ultricies enim eu sodales aliquet.' )</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="str">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( 'dffeab07-7872-4d13-aa6b-5480afb9b2d8','Grim Test','Nullam et tellus cursus, dapibus arcu et, blandit lacus.' )</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="str">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( 'ec68bfed-f064-422b-94c6-ab817f5e0dd8','Straw Donut','In nec neque sit amet mi tempor suscipit.' )</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
       <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="str">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( 'a8b08005-3d10-4b7a-b4b9-6df523c8ae07','Dreadful Nitrogen','Ut suscipit augue vel facilisis fermentum.' )</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="str">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( '137255ed-78f0-4f31-abbb-6759486938f0','Sticky Ray','Ut convallis orci nec ligula condimentum, sed pretium urna ullamcorper.' )</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Implemented a skeleton BLL to test against
</commit_message>
<xml_diff>
--- a/UT.Vend.BLL/HelperFiles/Project.xlsx
+++ b/UT.Vend.BLL/HelperFiles/Project.xlsx
@@ -240,7 +240,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -296,8 +296,8 @@
         <v>1</v>
       </c>
       <c r="G2" s="0" t="str">
-        <f aca="false">"INSERT INTO "&amp;A2&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "' )"</f>
-        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( 'f79359bb-2524-4cd5-b452-acaa8fd0d33b','Scorpion Cloudy','Lorem ipsum dolor sit amet, consectetur adipiscing elit.' )</v>
+        <f aca="false">"INSERT INTO "&amp;A2&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "' ,'" &amp; E2 &amp; "','" &amp; F2 &amp; "')"</f>
+        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc],[AddrID],[ActiveFlg]) VALUES ( 'f79359bb-2524-4cd5-b452-acaa8fd0d33b','Scorpion Cloudy','Lorem ipsum dolor sit amet, consectetur adipiscing elit.' ,'9','1')</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -320,8 +320,8 @@
         <v>1</v>
       </c>
       <c r="G3" s="0" t="str">
-        <f aca="false">"INSERT INTO "&amp;A3&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "','" &amp; D3 &amp; "' )"</f>
-        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( '5cc9ad09-3002-40e8-8a30-96b656a9d805','Minimum Bulldozer','Praesent varius dolor quis sollicitudin ornare.' )</v>
+        <f aca="false">"INSERT INTO "&amp;A3&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "','" &amp; D3 &amp; "' ,'" &amp; E3 &amp; "','" &amp; F3 &amp; "')"</f>
+        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc],[AddrID],[ActiveFlg]) VALUES ( '5cc9ad09-3002-40e8-8a30-96b656a9d805','Minimum Bulldozer','Praesent varius dolor quis sollicitudin ornare.' ,'6','1')</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -344,8 +344,8 @@
         <v>1</v>
       </c>
       <c r="G4" s="0" t="str">
-        <f aca="false">"INSERT INTO "&amp;A4&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B4 &amp; "','" &amp; C4 &amp; "','" &amp; D4 &amp; "' )"</f>
-        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( '54dbcf7a-0328-4a8d-9562-7d8c8b0c930b','Grotesque Viper','Duis a neque ac est fermentum rhoncus ac sed quam.' )</v>
+        <f aca="false">"INSERT INTO "&amp;A4&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B4 &amp; "','" &amp; C4 &amp; "','" &amp; D4 &amp; "' ,'" &amp; E4 &amp; "','" &amp; F4 &amp; "')"</f>
+        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc],[AddrID],[ActiveFlg]) VALUES ( '54dbcf7a-0328-4a8d-9562-7d8c8b0c930b','Grotesque Viper','Duis a neque ac est fermentum rhoncus ac sed quam.' ,'2','1')</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -368,8 +368,8 @@
         <v>1</v>
       </c>
       <c r="G5" s="0" t="str">
-        <f aca="false">"INSERT INTO "&amp;A5&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B5 &amp; "','" &amp; C5 &amp; "','" &amp; D5 &amp; "' )"</f>
-        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( '364ac77c-d08e-4134-9849-fe731b00af2d','Wild Oyster','Sed ac quam vulputate, consectetur libero in, rutrum justo.' )</v>
+        <f aca="false">"INSERT INTO "&amp;A5&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B5 &amp; "','" &amp; C5 &amp; "','" &amp; D5 &amp; "' ,'" &amp; E5 &amp; "','" &amp; F5 &amp; "')"</f>
+        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc],[AddrID],[ActiveFlg]) VALUES ( '364ac77c-d08e-4134-9849-fe731b00af2d','Wild Oyster','Sed ac quam vulputate, consectetur libero in, rutrum justo.' ,'7','1')</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -392,8 +392,8 @@
         <v>1</v>
       </c>
       <c r="G6" s="0" t="str">
-        <f aca="false">"INSERT INTO "&amp;A6&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B6 &amp; "','" &amp; C6 &amp; "','" &amp; D6 &amp; "' )"</f>
-        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( '25c7f719-8bde-447c-9b53-226c612de0bb','Third Temporary Hook','Nunc nec ipsum vitae ligula rutrum laoreet.' )</v>
+        <f aca="false">"INSERT INTO "&amp;A6&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B6 &amp; "','" &amp; C6 &amp; "','" &amp; D6 &amp; "' ,'" &amp; E6 &amp; "','" &amp; F6 &amp; "')"</f>
+        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc],[AddrID],[ActiveFlg]) VALUES ( '25c7f719-8bde-447c-9b53-226c612de0bb','Third Temporary Hook','Nunc nec ipsum vitae ligula rutrum laoreet.' ,'7','1')</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,8 +416,8 @@
         <v>1</v>
       </c>
       <c r="G7" s="0" t="str">
-        <f aca="false">"INSERT INTO "&amp;A7&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B7 &amp; "','" &amp; C7 &amp; "','" &amp; D7 &amp; "' )"</f>
-        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( 'fb986b83-d3c1-4dc6-bb25-4ddc3423fd5e','Mysterious Fish','Nam ultricies enim eu sodales aliquet.' )</v>
+        <f aca="false">"INSERT INTO "&amp;A7&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B7 &amp; "','" &amp; C7 &amp; "','" &amp; D7 &amp; "' ,'" &amp; E7 &amp; "','" &amp; F7 &amp; "')"</f>
+        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc],[AddrID],[ActiveFlg]) VALUES ( 'fb986b83-d3c1-4dc6-bb25-4ddc3423fd5e','Mysterious Fish','Nam ultricies enim eu sodales aliquet.' ,'6','1')</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,8 +440,8 @@
         <v>1</v>
       </c>
       <c r="G8" s="0" t="str">
-        <f aca="false">"INSERT INTO "&amp;A8&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B8 &amp; "','" &amp; C8 &amp; "','" &amp; D8 &amp; "' )"</f>
-        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( 'dffeab07-7872-4d13-aa6b-5480afb9b2d8','Grim Test','Nullam et tellus cursus, dapibus arcu et, blandit lacus.' )</v>
+        <f aca="false">"INSERT INTO "&amp;A8&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B8 &amp; "','" &amp; C8 &amp; "','" &amp; D8 &amp; "' ,'" &amp; E8 &amp; "','" &amp; F8 &amp; "')"</f>
+        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc],[AddrID],[ActiveFlg]) VALUES ( 'dffeab07-7872-4d13-aa6b-5480afb9b2d8','Grim Test','Nullam et tellus cursus, dapibus arcu et, blandit lacus.' ,'3','1')</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,8 +464,8 @@
         <v>1</v>
       </c>
       <c r="G9" s="0" t="str">
-        <f aca="false">"INSERT INTO "&amp;A9&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B9 &amp; "','" &amp; C9 &amp; "','" &amp; D9 &amp; "' )"</f>
-        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( 'ec68bfed-f064-422b-94c6-ab817f5e0dd8','Straw Donut','In nec neque sit amet mi tempor suscipit.' )</v>
+        <f aca="false">"INSERT INTO "&amp;A9&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B9 &amp; "','" &amp; C9 &amp; "','" &amp; D9 &amp; "' ,'" &amp; E9 &amp; "','" &amp; F9 &amp; "')"</f>
+        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc],[AddrID],[ActiveFlg]) VALUES ( 'ec68bfed-f064-422b-94c6-ab817f5e0dd8','Straw Donut','In nec neque sit amet mi tempor suscipit.' ,'3','1')</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,8 +488,8 @@
         <v>1</v>
       </c>
       <c r="G10" s="0" t="str">
-        <f aca="false">"INSERT INTO "&amp;A10&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B10 &amp; "','" &amp; C10 &amp; "','" &amp; D10 &amp; "' )"</f>
-        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( 'a8b08005-3d10-4b7a-b4b9-6df523c8ae07','Dreadful Nitrogen','Ut suscipit augue vel facilisis fermentum.' )</v>
+        <f aca="false">"INSERT INTO "&amp;A10&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B10 &amp; "','" &amp; C10 &amp; "','" &amp; D10 &amp; "' ,'" &amp; E10 &amp; "','" &amp; F10 &amp; "')"</f>
+        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc],[AddrID],[ActiveFlg]) VALUES ( 'a8b08005-3d10-4b7a-b4b9-6df523c8ae07','Dreadful Nitrogen','Ut suscipit augue vel facilisis fermentum.' ,'6','1')</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,8 +512,8 @@
         <v>1</v>
       </c>
       <c r="G11" s="0" t="str">
-        <f aca="false">"INSERT INTO "&amp;A11&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"]) VALUES ( '" &amp; B11 &amp; "','" &amp; C11 &amp; "','" &amp; D11 &amp; "' )"</f>
-        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc]) VALUES ( '137255ed-78f0-4f31-abbb-6759486938f0','Sticky Ray','Ut convallis orci nec ligula condimentum, sed pretium urna ullamcorper.' )</v>
+        <f aca="false">"INSERT INTO "&amp;A11&amp;" ([" &amp; B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B11 &amp; "','" &amp; C11 &amp; "','" &amp; D11 &amp; "' ,'" &amp; E11 &amp; "','" &amp; F11 &amp; "')"</f>
+        <v>INSERT INTO [Vend].[tblProject] ([ProjectID],[ProjectName],[ProjectDesc],[AddrID],[ActiveFlg]) VALUES ( '137255ed-78f0-4f31-abbb-6759486938f0','Sticky Ray','Ut convallis orci nec ligula condimentum, sed pretium urna ullamcorper.' ,'4','1')</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>